<commit_message>
added labels for parameter screen, added 'Set all' button, fixed bug in modifying database
</commit_message>
<xml_diff>
--- a/database - copy.xlsx
+++ b/database - copy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Core\Programming\REPOS\Pacemaker-DCM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D60E616-ACC0-4FF8-B6D4-40F01D5D97F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED2E480-25CC-4B87-8994-7263C8F8E1B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7" yWindow="80" windowWidth="25520" windowHeight="13720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7" yWindow="80" windowWidth="25520" windowHeight="13720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="USERS" sheetId="2" r:id="rId1"/>
@@ -505,8 +505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09CB3C7F-CF6E-4F9D-9BB2-F3F03BC309F2}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -538,8 +538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F5AE9C5-FF3E-4CAE-B61D-60D3D3DFDA01}">
   <dimension ref="A1:AC1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.3515625" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>

</xml_diff>